<commit_message>
test all upload success
</commit_message>
<xml_diff>
--- a/ra_exploer/examples/LTS_TR2_All.xlsx
+++ b/ra_exploer/examples/LTS_TR2_All.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hp06316p\技術開發一部&amp;二部\技術開發一部\技術開發三課\個人暫存區\康良豪\RA選擇器\Summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dimsp\Documents\Projects\td_toolkits_reconstruc\ra_exploer\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63146EB3-024E-452D-8FEA-10B3B4A533C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7965"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTS" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="48">
   <si>
     <t>項目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,29 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>³</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Bulk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -151,29 +129,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>³</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>723K1M</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -234,29 +189,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>³</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>10</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LCT-15-1098</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -278,75 +210,6 @@
   </si>
   <si>
     <t>Test Cell</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>³</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>³</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>³</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>12</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -367,29 +230,6 @@
   </si>
   <si>
     <t>LCT-19-580</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>³</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>14</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -408,7 +248,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -460,9 +300,10 @@
     <font>
       <sz val="12"/>
       <color rgb="FF3333FF"/>
-      <name val="Symbol"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -512,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -562,6 +403,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -596,7 +440,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="圖片 1"/>
+        <xdr:cNvPr id="2" name="圖片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -634,7 +484,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="圖片 2"/>
+        <xdr:cNvPr id="3" name="圖片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -672,7 +528,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="圖片 3"/>
+        <xdr:cNvPr id="4" name="圖片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -960,11 +822,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1031,31 +893,31 @@
       <c r="D2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="8">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>15</v>
       </c>
       <c r="G2" s="10">
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" s="9">
         <v>-20</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
@@ -1066,31 +928,31 @@
       <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>20</v>
+      <c r="E3" s="17">
+        <v>10</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" s="10">
         <v>1</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I3" s="9">
         <v>-30</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>12</v>
@@ -1099,28 +961,28 @@
         <v>13</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="8">
         <v>7</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I4" s="9">
         <v>-40</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1131,31 +993,31 @@
         <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="17">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I5" s="9">
         <v>-30</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1163,104 +1025,104 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E6" s="8">
         <v>8</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G6" s="10">
         <v>1</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="9">
         <v>-40</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E7" s="8">
         <v>3</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G7" s="10">
         <v>1</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" s="9">
         <v>-50</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="E8" s="8">
+        <v>10</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="9">
         <v>-20</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1268,34 +1130,34 @@
         <v>11</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="8">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="G9" s="10">
         <v>1</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I9" s="9">
         <v>-30</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1303,7 +1165,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>13</v>
@@ -1315,57 +1177,57 @@
         <v>5</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I10" s="9">
         <v>-40</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="E11" s="8">
+        <v>10</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I11" s="9">
         <v>-30</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1373,34 +1235,34 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" s="8">
         <v>8</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G12" s="10">
         <v>1</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I12" s="9">
         <v>-40</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K12" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1408,34 +1270,34 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E13" s="8">
         <v>2</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G13" s="10">
         <v>1</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I13" s="9">
         <v>-50</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1446,16 +1308,16 @@
         <v>12</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="8">
+        <v>10</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>15</v>
       </c>
       <c r="G14" s="10">
         <v>0.95</v>
@@ -1467,30 +1329,30 @@
         <v>-20</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8">
+        <v>12</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="G15" s="10">
         <v>0.95</v>
@@ -1502,15 +1364,15 @@
         <v>-30</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>12</v>
@@ -1525,7 +1387,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="10">
         <v>0.95</v>
@@ -1537,10 +1399,10 @@
         <v>-40</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1548,19 +1410,19 @@
         <v>11</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="E17" s="8">
+        <v>10</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G17" s="10">
         <v>0.95</v>
@@ -1572,30 +1434,30 @@
         <v>-30</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>44</v>
+        <v>26</v>
+      </c>
+      <c r="E18" s="8">
+        <v>12</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G18" s="10">
         <v>0.95</v>
@@ -1607,10 +1469,10 @@
         <v>-40</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1621,16 +1483,16 @@
         <v>12</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E19" s="8">
         <v>2</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G19" s="10">
         <v>0.95</v>
@@ -1642,10 +1504,10 @@
         <v>-50</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1661,26 +1523,26 @@
       <c r="D20" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>20</v>
+      <c r="E20" s="8">
+        <v>10</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G20" s="10">
         <v>0.9</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I20" s="9">
         <v>-20</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1694,28 +1556,28 @@
         <v>13</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="8">
+        <v>12</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>38</v>
       </c>
       <c r="G21" s="10">
         <v>0.9</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I21" s="9">
         <v>-30</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1723,7 +1585,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>13</v>
@@ -1735,7 +1597,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" s="10">
         <v>0.9</v>
@@ -1747,10 +1609,10 @@
         <v>-40</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1761,16 +1623,16 @@
         <v>12</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="E23" s="8">
+        <v>10</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G23" s="10">
         <v>0.9</v>
@@ -1782,30 +1644,30 @@
         <v>-30</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>45</v>
+        <v>26</v>
+      </c>
+      <c r="E24" s="8">
+        <v>12</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G24" s="10">
         <v>0.9</v>
@@ -1817,10 +1679,10 @@
         <v>-40</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1828,19 +1690,19 @@
         <v>11</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E25" s="8">
         <v>2</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G25" s="10">
         <v>0.9</v>
@@ -1852,15 +1714,15 @@
         <v>-50</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>12</v>
@@ -1871,11 +1733,11 @@
       <c r="D26" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>20</v>
+      <c r="E26" s="8">
+        <v>10</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G26" s="10">
         <v>0.85</v>
@@ -1887,10 +1749,10 @@
         <v>-20</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1904,13 +1766,13 @@
         <v>13</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>45</v>
+        <v>22</v>
+      </c>
+      <c r="E27" s="17">
+        <v>12</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G27" s="10">
         <v>0.85</v>
@@ -1922,10 +1784,10 @@
         <v>-30</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1939,28 +1801,28 @@
         <v>13</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E28" s="8">
         <v>5</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G28" s="10">
         <v>0.85</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I28" s="9">
         <v>-40</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -1971,31 +1833,31 @@
         <v>12</v>
       </c>
       <c r="C29" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>14</v>
+      <c r="E29" s="8">
+        <v>10</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G29" s="10">
         <v>0.85</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I29" s="9">
         <v>-30</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -2003,34 +1865,34 @@
         <v>11</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>45</v>
+        <v>26</v>
+      </c>
+      <c r="E30" s="8">
+        <v>12</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G30" s="10">
         <v>0.85</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I30" s="9">
         <v>-40</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K30" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2038,19 +1900,19 @@
         <v>11</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="E31" s="8">
         <v>2</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G31" s="10">
         <v>0.85</v>
@@ -2062,18 +1924,18 @@
         <v>-50</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>13</v>
@@ -2085,7 +1947,7 @@
         <v>10</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G32" s="10">
         <v>1</v>
@@ -2097,18 +1959,18 @@
         <v>-30</v>
       </c>
       <c r="J32" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K32" s="14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>13</v>
@@ -2116,26 +1978,26 @@
       <c r="D33" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>51</v>
+      <c r="E33" s="13">
+        <v>14</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G33" s="10">
         <v>1</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I33" s="7">
         <v>-30</v>
       </c>
       <c r="J33" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2143,19 +2005,19 @@
         <v>11</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E34" s="13">
         <v>12</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G34" s="10">
         <v>1</v>
@@ -2167,10 +2029,10 @@
         <v>-30</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>